<commit_message>
Améliorations WhatsApp, analytics et extraction IA
Ajoute la correction automatique des sources WhatsApp, enrichit les statistiques et analytics (top clients, produits, tendances), améliore la gestion des clients et la détection des commandes WhatsApp. Le prompt d'extraction IA est renforcé pour la darija et l'arabe. Ajoute des scripts de correction (fix_phones.py, fix_source.py), de nouveaux endpoints API (notifications/check), et des statistiques détaillées sur l'intégration WhatsApp. Plusieurs templates et la base de données sont mis à jour pour supporter ces évolutions.
</commit_message>
<xml_diff>
--- a/exports/commandes.xlsx
+++ b/exports/commandes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Commandes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Commandes" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,26 +514,18 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>TEST-001</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Entreprise Test SARL</t>
+          <t>Atlas Pack</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sachets fond plat</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Sachets kraft 15x25cm</t>
-        </is>
-      </c>
+          <t>Sac fond carré avec poignées plates</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
         <v>5000</v>
       </c>
@@ -542,38 +534,26 @@
           <t>pièces</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>MAD</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2024-12-23</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>2025-01-15</t>
-        </is>
-      </c>
+          <t>2025-12-23</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>en_attente</t>
+          <t>validee</t>
         </is>
       </c>
       <c r="N2" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>2025-12-23 20:41:16</t>
+          <t>2025-12-27 21:11:39</t>
         </is>
       </c>
     </row>
@@ -581,32 +561,24 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-04</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Marjane Market</t>
+          <t>marjane market</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sac fond carré sans poignées</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Sacs Kraft Fond Carré (Format Standard)</t>
-        </is>
-      </c>
+          <t>Sachets fond plat</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>15000</v>
+        <v>600</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>unités</t>
+          <t>pièces</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -614,7 +586,7 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="L3" t="inlineStr"/>
@@ -624,11 +596,11 @@
         </is>
       </c>
       <c r="N3" t="n">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>2025-12-23 20:43:37</t>
+          <t>2025-12-27 22:14:09</t>
         </is>
       </c>
     </row>
@@ -639,7 +611,7 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Supermarché Nour</t>
+          <t>Opoint</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -649,11 +621,11 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>sacs fond carré en marron</t>
+          <t>sacs en cartonne pour les commandes de tacos</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -665,7 +637,7 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
+          <t>2025-12-27</t>
         </is>
       </c>
       <c r="L4" t="inlineStr"/>
@@ -675,11 +647,11 @@
         </is>
       </c>
       <c r="N4" t="n">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>2025-12-23 20:54:10</t>
+          <t>2025-12-27 22:37:51</t>
         </is>
       </c>
     </row>
@@ -690,21 +662,17 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ch'hiwat Fès</t>
+          <t>ecole centrale casablanca</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Sac fond carré avec poignées plates</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>sacs poignées plates (hadouk lli kano f le dernier échantillon)</t>
-        </is>
-      </c>
+          <t>Sachets fond plat</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -716,10 +684,14 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr"/>
+          <t>2025-12-27</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>2026-01-05</t>
+        </is>
+      </c>
       <c r="M5" t="inlineStr">
         <is>
           <t>en_attente</t>
@@ -730,7 +702,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>2025-12-23 21:03:50</t>
+          <t>2025-12-27 22:41:17</t>
         </is>
       </c>
     </row>
@@ -741,21 +713,21 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Ch'hiwat Fès</t>
+          <t>Client WhatsApp +212617087040</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sac fond carré avec poignées plates</t>
+          <t>Sachets fond plat</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>sacs poignées plates</t>
+          <t>black pack</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>8000</v>
+        <v>5000</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -767,266 +739,25 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2025-12-23</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr"/>
+          <t>2025-12-27</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>2026-01-05</t>
+        </is>
+      </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>en_attente</t>
         </is>
       </c>
       <c r="N6" t="n">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>2025-12-23 21:07:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Société Atlas Pack</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Sac fond carré sans poignées</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Format 25x30 avec impression logo en 2 couleurs</t>
-        </is>
-      </c>
-      <c r="F7" t="n">
-        <v>12000</v>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>pièces</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>2025-12-23</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>en_attente</t>
-        </is>
-      </c>
-      <c r="N7" t="n">
-        <v>85</v>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>2025-12-23 21:08:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1096</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Marjane Market</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>2025-12-23</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>en_attente</t>
-        </is>
-      </c>
-      <c r="N8" t="n">
-        <v>50</v>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>2025-12-23 21:35:05</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>chhiwat fes</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Sac fond carré avec poignées plates</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>sacs poignées plates</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>8000</v>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>pièces</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>2025-12-23</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>en_attente</t>
-        </is>
-      </c>
-      <c r="N9" t="n">
-        <v>85</v>
-      </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>2025-12-23 22:01:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>chhiwat fes</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Sac fond carré avec poignées plates</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>sacs poignées plates</t>
-        </is>
-      </c>
-      <c r="F10" t="n">
-        <v>8000</v>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>pièces</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>2025-12-23</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>en_attente</t>
-        </is>
-      </c>
-      <c r="N10" t="n">
-        <v>85</v>
-      </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>2025-12-23 22:02:01</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>marjane market</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Sac fond carré sans poignées</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Sacs Kraft Fond Carré (Format Standard)</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>15000</v>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>unités</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>2025-12-23</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>en_attente</t>
-        </is>
-      </c>
-      <c r="N11" t="n">
-        <v>85</v>
-      </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>2025-12-23 22:02:05</t>
+          <t>2025-12-27 22:52:57</t>
         </is>
       </c>
     </row>

</xml_diff>